<commit_message>
Deleted 3 files.  Linked 3 tests to Spira via GitHub
</commit_message>
<xml_diff>
--- a/MxMasterTest/MxNavigation/b2000-MyAccount/Main.rvl.xlsx
+++ b/MxMasterTest/MxNavigation/b2000-MyAccount/Main.rvl.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="21">
   <si>
     <t>Flow</t>
   </si>
@@ -533,7 +533,7 @@
         <v>16</v>
       </c>
       <c r="G4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5">

</xml_diff>